<commit_message>
etc/: Use PLC data types in delta spreadsheets
Use PLC data types instead of directly naming record
data types in delta ioc example spreadsheets.
</commit_message>
<xml_diff>
--- a/etc/delta_example_style_1.xlsx
+++ b/etc/delta_example_style_1.xlsx
@@ -5,19 +5,22 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Delta" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$O$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$O$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!$A$1:$O$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$O$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$O$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$O$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$O$1</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Delta!$A$1:$O$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Delta!$A$1:$O$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Delta!$A$1:$O$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Delta!$A$1:$O$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Delta!$A$1:$O$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Delta!$A$1:$O$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Delta!$A$1:$O$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Delta!$A$1:$O$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">Delta!$A$1:$O$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">Delta!$A$1:$O$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -29,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="262">
   <si>
     <t xml:space="preserve">Nº</t>
   </si>
@@ -100,7 +103,7 @@
     <t xml:space="preserve">Mon</t>
   </si>
   <si>
-    <t xml:space="preserve">Digital</t>
+    <t xml:space="preserve">Bit</t>
   </si>
   <si>
     <t xml:space="preserve">Input</t>
@@ -196,7 +199,7 @@
     <t xml:space="preserve">Sel</t>
   </si>
   <si>
-    <t xml:space="preserve">Control</t>
+    <t xml:space="preserve">Output</t>
   </si>
   <si>
     <t xml:space="preserve">EnFlags[0]</t>
@@ -322,10 +325,7 @@
     <t xml:space="preserve">SP</t>
   </si>
   <si>
-    <t xml:space="preserve">Analog</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Output</t>
+    <t xml:space="preserve">Real</t>
   </si>
   <si>
     <t xml:space="preserve">mm/s2</t>
@@ -1224,31 +1224,31 @@
   <dimension ref="1:84"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I84" activeCellId="0" sqref="I84"/>
+      <selection pane="bottomLeft" activeCell="B79" activeCellId="0" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="34.1428571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="7.79591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="4" width="8.14285714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="7.62244897959184"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="4" width="20.1428571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="37.8877551020408"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="7" width="12.75"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="7" width="10.3112244897959"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="8.31632653061224"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="7" width="30.0561224489796"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="8" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="9" width="4.84183673469388"/>
-    <col collapsed="false" hidden="false" max="1023" min="17" style="9" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.0969387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="48.9591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="10.9795918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="4" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="4" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="4" width="16.3775510204082"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="4" width="28.7959183673469"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="16.3775510204082"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="6" width="54.3571428571429"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="7" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="7" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="7" width="11.6989795918367"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="7" width="43.015306122449"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="8" width="16.3775510204082"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="9" width="6.65816326530612"/>
+    <col collapsed="false" hidden="false" max="1023" min="17" style="9" width="26.0969387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="17.6377551020408"/>
   </cols>
   <sheetData>
     <row r="1" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2563,10 +2563,10 @@
         <v>97</v>
       </c>
       <c r="L27" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="M27" s="22" t="s">
         <v>98</v>
-      </c>
-      <c r="M27" s="22" t="s">
-        <v>99</v>
       </c>
       <c r="N27" s="22" t="s">
         <v>95</v>
@@ -2583,25 +2583,25 @@
         <v>27</v>
       </c>
       <c r="B28" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="C28" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="19" t="s">
         <v>100</v>
-      </c>
-      <c r="C28" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D28" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E28" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G28" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H28" s="19" t="s">
-        <v>101</v>
       </c>
       <c r="I28" s="20" t="s">
         <v>96</v>
@@ -2614,13 +2614,13 @@
         <v>97</v>
       </c>
       <c r="L28" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M28" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N28" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O28" s="23" t="s">
         <v>25</v>
@@ -2634,25 +2634,25 @@
         <v>28</v>
       </c>
       <c r="B29" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H29" s="19" t="s">
         <v>103</v>
-      </c>
-      <c r="C29" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D29" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E29" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F29" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G29" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H29" s="19" t="s">
-        <v>104</v>
       </c>
       <c r="I29" s="20" t="s">
         <v>96</v>
@@ -2665,13 +2665,13 @@
         <v>97</v>
       </c>
       <c r="L29" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M29" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N29" s="22" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="O29" s="23" t="s">
         <v>25</v>
@@ -2685,25 +2685,25 @@
         <v>29</v>
       </c>
       <c r="B30" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="C30" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" s="19" t="s">
         <v>106</v>
-      </c>
-      <c r="C30" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F30" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G30" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H30" s="19" t="s">
-        <v>107</v>
       </c>
       <c r="I30" s="20" t="s">
         <v>96</v>
@@ -2716,13 +2716,13 @@
         <v>97</v>
       </c>
       <c r="L30" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="M30" s="22" t="s">
         <v>98</v>
       </c>
-      <c r="M30" s="22" t="s">
-        <v>99</v>
-      </c>
       <c r="N30" s="22" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O30" s="23" t="s">
         <v>25</v>
@@ -2736,25 +2736,25 @@
         <v>30</v>
       </c>
       <c r="B31" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H31" s="19" t="s">
         <v>108</v>
-      </c>
-      <c r="C31" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E31" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F31" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G31" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H31" s="19" t="s">
-        <v>109</v>
       </c>
       <c r="I31" s="20" t="s">
         <v>96</v>
@@ -2767,13 +2767,13 @@
         <v>97</v>
       </c>
       <c r="L31" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M31" s="22" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N31" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O31" s="23" t="s">
         <v>25</v>
@@ -2787,25 +2787,25 @@
         <v>31</v>
       </c>
       <c r="B32" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H32" s="19" t="s">
         <v>110</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E32" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F32" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G32" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H32" s="19" t="s">
-        <v>111</v>
       </c>
       <c r="I32" s="20" t="s">
         <v>96</v>
@@ -2818,13 +2818,13 @@
         <v>97</v>
       </c>
       <c r="L32" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M32" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N32" s="22" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O32" s="23" t="s">
         <v>25</v>
@@ -2838,25 +2838,25 @@
         <v>32</v>
       </c>
       <c r="B33" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="C33" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H33" s="19" t="s">
         <v>112</v>
-      </c>
-      <c r="C33" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E33" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F33" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G33" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H33" s="19" t="s">
-        <v>113</v>
       </c>
       <c r="I33" s="20" t="s">
         <v>96</v>
@@ -2869,13 +2869,13 @@
         <v>97</v>
       </c>
       <c r="L33" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M33" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N33" s="22" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O33" s="23" t="s">
         <v>25</v>
@@ -2889,25 +2889,25 @@
         <v>33</v>
       </c>
       <c r="B34" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" s="19" t="s">
         <v>115</v>
-      </c>
-      <c r="C34" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E34" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F34" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G34" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H34" s="19" t="s">
-        <v>116</v>
       </c>
       <c r="I34" s="20" t="s">
         <v>96</v>
@@ -2920,13 +2920,13 @@
         <v>97</v>
       </c>
       <c r="L34" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M34" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N34" s="22" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O34" s="23" t="s">
         <v>25</v>
@@ -2940,25 +2940,25 @@
         <v>34</v>
       </c>
       <c r="B35" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F35" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H35" s="19" t="s">
         <v>117</v>
-      </c>
-      <c r="C35" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D35" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E35" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F35" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G35" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H35" s="19" t="s">
-        <v>118</v>
       </c>
       <c r="I35" s="20" t="s">
         <v>96</v>
@@ -2971,11 +2971,11 @@
         <v>97</v>
       </c>
       <c r="L35" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M35" s="22"/>
       <c r="N35" s="22" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="O35" s="23" t="s">
         <v>25</v>
@@ -2989,25 +2989,25 @@
         <v>35</v>
       </c>
       <c r="B36" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F36" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G36" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H36" s="19" t="s">
         <v>119</v>
-      </c>
-      <c r="C36" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D36" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E36" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F36" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G36" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H36" s="19" t="s">
-        <v>120</v>
       </c>
       <c r="I36" s="20" t="s">
         <v>96</v>
@@ -3020,11 +3020,11 @@
         <v>97</v>
       </c>
       <c r="L36" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M36" s="22"/>
       <c r="N36" s="22" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O36" s="23" t="s">
         <v>25</v>
@@ -3038,25 +3038,25 @@
         <v>36</v>
       </c>
       <c r="B37" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="C37" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F37" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H37" s="19" t="s">
         <v>121</v>
-      </c>
-      <c r="C37" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D37" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E37" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F37" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G37" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H37" s="19" t="s">
-        <v>122</v>
       </c>
       <c r="I37" s="20" t="s">
         <v>22</v>
@@ -3069,13 +3069,13 @@
         <v>97</v>
       </c>
       <c r="L37" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M37" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N37" s="22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="O37" s="23" t="s">
         <v>25</v>
@@ -3089,25 +3089,25 @@
         <v>37</v>
       </c>
       <c r="B38" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="C38" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G38" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H38" s="19" t="s">
         <v>124</v>
-      </c>
-      <c r="C38" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D38" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E38" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F38" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G38" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H38" s="19" t="s">
-        <v>125</v>
       </c>
       <c r="I38" s="20" t="s">
         <v>22</v>
@@ -3120,13 +3120,13 @@
         <v>97</v>
       </c>
       <c r="L38" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M38" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N38" s="22" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="O38" s="23" t="s">
         <v>25</v>
@@ -3140,25 +3140,25 @@
         <v>38</v>
       </c>
       <c r="B39" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C39" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G39" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H39" s="19" t="s">
         <v>127</v>
-      </c>
-      <c r="C39" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D39" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E39" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F39" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G39" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H39" s="19" t="s">
-        <v>128</v>
       </c>
       <c r="I39" s="20" t="s">
         <v>22</v>
@@ -3171,13 +3171,13 @@
         <v>97</v>
       </c>
       <c r="L39" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M39" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="N39" s="22" t="s">
         <v>129</v>
-      </c>
-      <c r="N39" s="22" t="s">
-        <v>130</v>
       </c>
       <c r="O39" s="23" t="s">
         <v>25</v>
@@ -3191,25 +3191,25 @@
         <v>39</v>
       </c>
       <c r="B40" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="C40" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F40" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G40" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H40" s="19" t="s">
         <v>131</v>
-      </c>
-      <c r="C40" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E40" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F40" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G40" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H40" s="19" t="s">
-        <v>132</v>
       </c>
       <c r="I40" s="20" t="s">
         <v>22</v>
@@ -3222,13 +3222,13 @@
         <v>97</v>
       </c>
       <c r="L40" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M40" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N40" s="22" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="O40" s="23" t="s">
         <v>25</v>
@@ -3242,25 +3242,25 @@
         <v>40</v>
       </c>
       <c r="B41" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="C41" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E41" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F41" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G41" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H41" s="19" t="s">
         <v>134</v>
-      </c>
-      <c r="C41" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D41" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E41" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F41" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G41" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H41" s="19" t="s">
-        <v>135</v>
       </c>
       <c r="I41" s="20" t="s">
         <v>22</v>
@@ -3273,13 +3273,13 @@
         <v>97</v>
       </c>
       <c r="L41" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M41" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N41" s="22" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="O41" s="23" t="s">
         <v>25</v>
@@ -3293,25 +3293,25 @@
         <v>41</v>
       </c>
       <c r="B42" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E42" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F42" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G42" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H42" s="19" t="s">
         <v>137</v>
-      </c>
-      <c r="C42" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E42" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F42" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G42" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H42" s="19" t="s">
-        <v>138</v>
       </c>
       <c r="I42" s="20" t="s">
         <v>22</v>
@@ -3328,7 +3328,7 @@
       </c>
       <c r="M42" s="22"/>
       <c r="N42" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="O42" s="23" t="s">
         <v>25</v>
@@ -3342,25 +3342,25 @@
         <v>42</v>
       </c>
       <c r="B43" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C43" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F43" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G43" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H43" s="19" t="s">
         <v>140</v>
-      </c>
-      <c r="C43" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D43" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E43" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F43" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G43" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H43" s="19" t="s">
-        <v>141</v>
       </c>
       <c r="I43" s="20" t="s">
         <v>22</v>
@@ -3377,7 +3377,7 @@
       </c>
       <c r="M43" s="22"/>
       <c r="N43" s="22" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="O43" s="23" t="s">
         <v>25</v>
@@ -3391,25 +3391,25 @@
         <v>43</v>
       </c>
       <c r="B44" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="C44" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E44" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F44" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G44" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H44" s="19" t="s">
         <v>143</v>
-      </c>
-      <c r="C44" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D44" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E44" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F44" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G44" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H44" s="19" t="s">
-        <v>144</v>
       </c>
       <c r="I44" s="20" t="s">
         <v>22</v>
@@ -3426,7 +3426,7 @@
       </c>
       <c r="M44" s="22"/>
       <c r="N44" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="O44" s="23" t="s">
         <v>25</v>
@@ -3440,25 +3440,25 @@
         <v>44</v>
       </c>
       <c r="B45" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="C45" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D45" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E45" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G45" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H45" s="19" t="s">
         <v>146</v>
-      </c>
-      <c r="C45" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D45" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E45" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F45" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G45" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H45" s="19" t="s">
-        <v>147</v>
       </c>
       <c r="I45" s="20" t="s">
         <v>96</v>
@@ -3471,13 +3471,13 @@
         <v>97</v>
       </c>
       <c r="L45" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M45" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N45" s="22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="O45" s="23" t="s">
         <v>25</v>
@@ -3491,25 +3491,25 @@
         <v>45</v>
       </c>
       <c r="B46" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="C46" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D46" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E46" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F46" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G46" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H46" s="19" t="s">
         <v>149</v>
-      </c>
-      <c r="C46" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D46" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E46" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F46" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G46" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H46" s="19" t="s">
-        <v>150</v>
       </c>
       <c r="I46" s="20" t="s">
         <v>54</v>
@@ -3526,7 +3526,7 @@
       </c>
       <c r="M46" s="22"/>
       <c r="N46" s="22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="O46" s="23" t="s">
         <v>25</v>
@@ -3540,25 +3540,25 @@
         <v>46</v>
       </c>
       <c r="B47" s="17" t="s">
+        <v>151</v>
+      </c>
+      <c r="C47" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D47" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E47" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F47" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G47" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H47" s="19" t="s">
         <v>152</v>
-      </c>
-      <c r="C47" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D47" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E47" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F47" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G47" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H47" s="19" t="s">
-        <v>153</v>
       </c>
       <c r="I47" s="20" t="s">
         <v>96</v>
@@ -3571,13 +3571,13 @@
         <v>97</v>
       </c>
       <c r="L47" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M47" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N47" s="22" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="O47" s="23" t="s">
         <v>25</v>
@@ -3591,25 +3591,25 @@
         <v>47</v>
       </c>
       <c r="B48" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="C48" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D48" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F48" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G48" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H48" s="19" t="s">
         <v>155</v>
-      </c>
-      <c r="C48" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D48" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E48" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F48" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G48" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H48" s="19" t="s">
-        <v>156</v>
       </c>
       <c r="I48" s="20" t="s">
         <v>22</v>
@@ -3622,13 +3622,13 @@
         <v>97</v>
       </c>
       <c r="L48" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M48" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N48" s="22" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="O48" s="23" t="s">
         <v>25</v>
@@ -3642,25 +3642,25 @@
         <v>48</v>
       </c>
       <c r="B49" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="C49" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D49" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E49" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F49" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G49" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H49" s="19" t="s">
         <v>158</v>
-      </c>
-      <c r="C49" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D49" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E49" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F49" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G49" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H49" s="19" t="s">
-        <v>159</v>
       </c>
       <c r="I49" s="20" t="s">
         <v>22</v>
@@ -3673,13 +3673,13 @@
         <v>97</v>
       </c>
       <c r="L49" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M49" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N49" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O49" s="23" t="s">
         <v>25</v>
@@ -3693,25 +3693,25 @@
         <v>49</v>
       </c>
       <c r="B50" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="C50" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D50" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E50" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F50" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G50" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H50" s="19" t="s">
         <v>161</v>
-      </c>
-      <c r="C50" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D50" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E50" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F50" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G50" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H50" s="19" t="s">
-        <v>162</v>
       </c>
       <c r="I50" s="20" t="s">
         <v>22</v>
@@ -3724,13 +3724,13 @@
         <v>97</v>
       </c>
       <c r="L50" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M50" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N50" s="22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="O50" s="23" t="s">
         <v>25</v>
@@ -3744,25 +3744,25 @@
         <v>50</v>
       </c>
       <c r="B51" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="C51" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D51" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E51" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F51" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G51" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H51" s="19" t="s">
         <v>164</v>
-      </c>
-      <c r="C51" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D51" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E51" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F51" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G51" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H51" s="19" t="s">
-        <v>165</v>
       </c>
       <c r="I51" s="20" t="s">
         <v>22</v>
@@ -3775,13 +3775,13 @@
         <v>97</v>
       </c>
       <c r="L51" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M51" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N51" s="22" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="O51" s="23" t="s">
         <v>25</v>
@@ -3795,25 +3795,25 @@
         <v>51</v>
       </c>
       <c r="B52" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="C52" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D52" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E52" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F52" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G52" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H52" s="19" t="s">
         <v>167</v>
-      </c>
-      <c r="C52" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D52" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E52" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F52" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G52" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H52" s="19" t="s">
-        <v>168</v>
       </c>
       <c r="I52" s="20" t="s">
         <v>22</v>
@@ -3826,13 +3826,13 @@
         <v>97</v>
       </c>
       <c r="L52" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M52" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N52" s="22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="O52" s="23" t="s">
         <v>25</v>
@@ -3846,25 +3846,25 @@
         <v>52</v>
       </c>
       <c r="B53" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="C53" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D53" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E53" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F53" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G53" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H53" s="19" t="s">
         <v>170</v>
-      </c>
-      <c r="C53" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D53" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E53" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F53" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G53" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H53" s="19" t="s">
-        <v>171</v>
       </c>
       <c r="I53" s="20" t="s">
         <v>22</v>
@@ -3881,7 +3881,7 @@
       </c>
       <c r="M53" s="22"/>
       <c r="N53" s="22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="O53" s="23" t="s">
         <v>25</v>
@@ -3895,25 +3895,25 @@
         <v>53</v>
       </c>
       <c r="B54" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="C54" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D54" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E54" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F54" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G54" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H54" s="19" t="s">
         <v>173</v>
-      </c>
-      <c r="C54" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D54" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E54" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F54" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G54" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H54" s="19" t="s">
-        <v>174</v>
       </c>
       <c r="I54" s="20" t="s">
         <v>22</v>
@@ -3930,7 +3930,7 @@
       </c>
       <c r="M54" s="22"/>
       <c r="N54" s="22" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="O54" s="23" t="s">
         <v>25</v>
@@ -3944,25 +3944,25 @@
         <v>54</v>
       </c>
       <c r="B55" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="C55" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D55" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E55" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F55" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G55" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H55" s="19" t="s">
         <v>176</v>
-      </c>
-      <c r="C55" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D55" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E55" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F55" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G55" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H55" s="19" t="s">
-        <v>177</v>
       </c>
       <c r="I55" s="20" t="s">
         <v>22</v>
@@ -3979,7 +3979,7 @@
       </c>
       <c r="M55" s="22"/>
       <c r="N55" s="22" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="O55" s="23" t="s">
         <v>25</v>
@@ -3993,25 +3993,25 @@
         <v>55</v>
       </c>
       <c r="B56" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="C56" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E56" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F56" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G56" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H56" s="19" t="s">
         <v>179</v>
-      </c>
-      <c r="C56" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D56" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E56" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F56" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G56" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H56" s="19" t="s">
-        <v>180</v>
       </c>
       <c r="I56" s="20" t="s">
         <v>96</v>
@@ -4024,13 +4024,13 @@
         <v>97</v>
       </c>
       <c r="L56" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M56" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N56" s="22" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="O56" s="23" t="s">
         <v>25</v>
@@ -4044,25 +4044,25 @@
         <v>56</v>
       </c>
       <c r="B57" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="C57" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D57" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E57" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F57" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G57" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H57" s="19" t="s">
         <v>182</v>
-      </c>
-      <c r="C57" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D57" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E57" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F57" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G57" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H57" s="19" t="s">
-        <v>183</v>
       </c>
       <c r="I57" s="20" t="s">
         <v>54</v>
@@ -4079,7 +4079,7 @@
       </c>
       <c r="M57" s="22"/>
       <c r="N57" s="22" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="O57" s="23" t="s">
         <v>25</v>
@@ -4093,25 +4093,25 @@
         <v>57</v>
       </c>
       <c r="B58" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="C58" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D58" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E58" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F58" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G58" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H58" s="19" t="s">
         <v>185</v>
-      </c>
-      <c r="C58" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D58" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E58" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F58" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G58" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H58" s="19" t="s">
-        <v>186</v>
       </c>
       <c r="I58" s="20" t="s">
         <v>96</v>
@@ -4124,13 +4124,13 @@
         <v>97</v>
       </c>
       <c r="L58" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M58" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N58" s="22" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="O58" s="23" t="s">
         <v>25</v>
@@ -4144,25 +4144,25 @@
         <v>58</v>
       </c>
       <c r="B59" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="C59" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D59" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E59" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F59" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G59" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H59" s="19" t="s">
         <v>188</v>
-      </c>
-      <c r="C59" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D59" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E59" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F59" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G59" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H59" s="19" t="s">
-        <v>189</v>
       </c>
       <c r="I59" s="20" t="s">
         <v>22</v>
@@ -4175,13 +4175,13 @@
         <v>97</v>
       </c>
       <c r="L59" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M59" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N59" s="22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O59" s="23" t="s">
         <v>25</v>
@@ -4195,25 +4195,25 @@
         <v>59</v>
       </c>
       <c r="B60" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D60" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E60" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F60" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G60" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H60" s="19" t="s">
         <v>191</v>
-      </c>
-      <c r="C60" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D60" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E60" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F60" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G60" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H60" s="19" t="s">
-        <v>192</v>
       </c>
       <c r="I60" s="20" t="s">
         <v>22</v>
@@ -4226,13 +4226,13 @@
         <v>97</v>
       </c>
       <c r="L60" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M60" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N60" s="22" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="O60" s="23" t="s">
         <v>25</v>
@@ -4246,25 +4246,25 @@
         <v>60</v>
       </c>
       <c r="B61" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="C61" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D61" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E61" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F61" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G61" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H61" s="19" t="s">
         <v>194</v>
-      </c>
-      <c r="C61" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D61" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E61" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F61" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G61" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H61" s="19" t="s">
-        <v>195</v>
       </c>
       <c r="I61" s="20" t="s">
         <v>22</v>
@@ -4277,13 +4277,13 @@
         <v>97</v>
       </c>
       <c r="L61" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M61" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N61" s="22" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O61" s="23" t="s">
         <v>25</v>
@@ -4297,25 +4297,25 @@
         <v>61</v>
       </c>
       <c r="B62" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D62" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E62" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F62" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G62" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H62" s="19" t="s">
         <v>197</v>
-      </c>
-      <c r="C62" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D62" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E62" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F62" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G62" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H62" s="19" t="s">
-        <v>198</v>
       </c>
       <c r="I62" s="20" t="s">
         <v>22</v>
@@ -4328,13 +4328,13 @@
         <v>97</v>
       </c>
       <c r="L62" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M62" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N62" s="22" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="O62" s="23" t="s">
         <v>25</v>
@@ -4348,25 +4348,25 @@
         <v>62</v>
       </c>
       <c r="B63" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="C63" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D63" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E63" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F63" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G63" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H63" s="19" t="s">
         <v>200</v>
-      </c>
-      <c r="C63" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D63" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E63" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F63" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G63" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H63" s="19" t="s">
-        <v>201</v>
       </c>
       <c r="I63" s="20" t="s">
         <v>22</v>
@@ -4379,13 +4379,13 @@
         <v>97</v>
       </c>
       <c r="L63" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M63" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N63" s="22" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O63" s="23" t="s">
         <v>25</v>
@@ -4399,25 +4399,25 @@
         <v>63</v>
       </c>
       <c r="B64" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="C64" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D64" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E64" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F64" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G64" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H64" s="19" t="s">
         <v>203</v>
-      </c>
-      <c r="C64" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D64" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E64" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F64" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G64" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H64" s="19" t="s">
-        <v>204</v>
       </c>
       <c r="I64" s="20" t="s">
         <v>22</v>
@@ -4434,7 +4434,7 @@
       </c>
       <c r="M64" s="22"/>
       <c r="N64" s="22" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="O64" s="23" t="s">
         <v>25</v>
@@ -4448,25 +4448,25 @@
         <v>64</v>
       </c>
       <c r="B65" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="C65" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D65" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E65" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F65" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G65" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H65" s="19" t="s">
         <v>206</v>
-      </c>
-      <c r="C65" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D65" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E65" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F65" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G65" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H65" s="19" t="s">
-        <v>207</v>
       </c>
       <c r="I65" s="20" t="s">
         <v>22</v>
@@ -4483,7 +4483,7 @@
       </c>
       <c r="M65" s="22"/>
       <c r="N65" s="22" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="O65" s="23" t="s">
         <v>25</v>
@@ -4497,25 +4497,25 @@
         <v>65</v>
       </c>
       <c r="B66" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="C66" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D66" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E66" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F66" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G66" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H66" s="19" t="s">
         <v>209</v>
-      </c>
-      <c r="C66" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D66" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E66" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F66" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G66" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H66" s="19" t="s">
-        <v>210</v>
       </c>
       <c r="I66" s="20" t="s">
         <v>22</v>
@@ -4532,7 +4532,7 @@
       </c>
       <c r="M66" s="22"/>
       <c r="N66" s="22" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="O66" s="23" t="s">
         <v>25</v>
@@ -4546,25 +4546,25 @@
         <v>66</v>
       </c>
       <c r="B67" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D67" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E67" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F67" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G67" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H67" s="19" t="s">
         <v>212</v>
-      </c>
-      <c r="C67" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D67" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E67" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F67" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G67" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H67" s="19" t="s">
-        <v>213</v>
       </c>
       <c r="I67" s="20" t="s">
         <v>96</v>
@@ -4577,13 +4577,13 @@
         <v>97</v>
       </c>
       <c r="L67" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M67" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N67" s="22" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="O67" s="23" t="s">
         <v>25</v>
@@ -4597,25 +4597,25 @@
         <v>67</v>
       </c>
       <c r="B68" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="C68" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D68" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E68" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F68" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G68" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H68" s="19" t="s">
         <v>215</v>
-      </c>
-      <c r="C68" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D68" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E68" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F68" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G68" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H68" s="19" t="s">
-        <v>216</v>
       </c>
       <c r="I68" s="20" t="s">
         <v>54</v>
@@ -4632,7 +4632,7 @@
       </c>
       <c r="M68" s="22"/>
       <c r="N68" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O68" s="23" t="s">
         <v>25</v>
@@ -4646,25 +4646,25 @@
         <v>68</v>
       </c>
       <c r="B69" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="C69" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D69" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E69" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F69" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G69" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H69" s="19" t="s">
         <v>218</v>
-      </c>
-      <c r="C69" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D69" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E69" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F69" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G69" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H69" s="19" t="s">
-        <v>219</v>
       </c>
       <c r="I69" s="20" t="s">
         <v>96</v>
@@ -4677,13 +4677,13 @@
         <v>97</v>
       </c>
       <c r="L69" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M69" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N69" s="22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="O69" s="23" t="s">
         <v>25</v>
@@ -4697,25 +4697,25 @@
         <v>69</v>
       </c>
       <c r="B70" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="C70" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D70" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E70" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F70" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G70" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H70" s="19" t="s">
         <v>221</v>
-      </c>
-      <c r="C70" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D70" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E70" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F70" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G70" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H70" s="19" t="s">
-        <v>222</v>
       </c>
       <c r="I70" s="20" t="s">
         <v>22</v>
@@ -4728,13 +4728,13 @@
         <v>97</v>
       </c>
       <c r="L70" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M70" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N70" s="22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O70" s="23" t="s">
         <v>25</v>
@@ -4748,25 +4748,25 @@
         <v>70</v>
       </c>
       <c r="B71" s="17" t="s">
+        <v>223</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D71" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E71" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F71" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G71" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H71" s="19" t="s">
         <v>224</v>
-      </c>
-      <c r="C71" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D71" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E71" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F71" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G71" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H71" s="19" t="s">
-        <v>225</v>
       </c>
       <c r="I71" s="20" t="s">
         <v>22</v>
@@ -4779,13 +4779,13 @@
         <v>97</v>
       </c>
       <c r="L71" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M71" s="22" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="N71" s="22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O71" s="23" t="s">
         <v>25</v>
@@ -4799,25 +4799,25 @@
         <v>71</v>
       </c>
       <c r="B72" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="C72" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D72" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E72" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F72" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G72" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H72" s="19" t="s">
         <v>227</v>
-      </c>
-      <c r="C72" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D72" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E72" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F72" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G72" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H72" s="19" t="s">
-        <v>228</v>
       </c>
       <c r="I72" s="20" t="s">
         <v>22</v>
@@ -4830,13 +4830,13 @@
         <v>97</v>
       </c>
       <c r="L72" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M72" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N72" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="O72" s="23" t="s">
         <v>25</v>
@@ -4850,25 +4850,25 @@
         <v>72</v>
       </c>
       <c r="B73" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="C73" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D73" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E73" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F73" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G73" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H73" s="19" t="s">
         <v>230</v>
-      </c>
-      <c r="C73" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D73" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E73" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F73" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G73" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H73" s="19" t="s">
-        <v>231</v>
       </c>
       <c r="I73" s="20" t="s">
         <v>22</v>
@@ -4881,13 +4881,13 @@
         <v>97</v>
       </c>
       <c r="L73" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M73" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N73" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O73" s="23" t="s">
         <v>25</v>
@@ -4901,25 +4901,25 @@
         <v>73</v>
       </c>
       <c r="B74" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="C74" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D74" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E74" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F74" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G74" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H74" s="19" t="s">
         <v>233</v>
-      </c>
-      <c r="C74" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D74" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E74" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F74" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G74" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H74" s="19" t="s">
-        <v>234</v>
       </c>
       <c r="I74" s="20" t="s">
         <v>22</v>
@@ -4932,13 +4932,13 @@
         <v>97</v>
       </c>
       <c r="L74" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M74" s="22" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N74" s="22" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="O74" s="23" t="s">
         <v>25</v>
@@ -4952,25 +4952,25 @@
         <v>74</v>
       </c>
       <c r="B75" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="C75" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D75" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E75" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F75" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G75" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H75" s="19" t="s">
         <v>236</v>
-      </c>
-      <c r="C75" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D75" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E75" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F75" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G75" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H75" s="19" t="s">
-        <v>237</v>
       </c>
       <c r="I75" s="20" t="s">
         <v>22</v>
@@ -4987,7 +4987,7 @@
       </c>
       <c r="M75" s="22"/>
       <c r="N75" s="22" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="O75" s="23" t="s">
         <v>25</v>
@@ -5001,25 +5001,25 @@
         <v>75</v>
       </c>
       <c r="B76" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="C76" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D76" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E76" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F76" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G76" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H76" s="19" t="s">
         <v>239</v>
-      </c>
-      <c r="C76" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D76" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E76" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F76" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G76" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H76" s="19" t="s">
-        <v>240</v>
       </c>
       <c r="I76" s="20" t="s">
         <v>22</v>
@@ -5036,7 +5036,7 @@
       </c>
       <c r="M76" s="22"/>
       <c r="N76" s="22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="O76" s="23" t="s">
         <v>25</v>
@@ -5050,25 +5050,25 @@
         <v>76</v>
       </c>
       <c r="B77" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="C77" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D77" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E77" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F77" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G77" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H77" s="19" t="s">
         <v>242</v>
-      </c>
-      <c r="C77" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D77" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E77" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F77" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G77" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H77" s="19" t="s">
-        <v>243</v>
       </c>
       <c r="I77" s="20" t="s">
         <v>22</v>
@@ -5085,7 +5085,7 @@
       </c>
       <c r="M77" s="22"/>
       <c r="N77" s="22" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O77" s="23" t="s">
         <v>25</v>
@@ -5099,25 +5099,25 @@
         <v>77</v>
       </c>
       <c r="B78" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="C78" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D78" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E78" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F78" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G78" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H78" s="19" t="s">
         <v>245</v>
-      </c>
-      <c r="C78" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D78" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E78" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F78" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G78" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H78" s="19" t="s">
-        <v>246</v>
       </c>
       <c r="I78" s="20" t="s">
         <v>96</v>
@@ -5130,13 +5130,13 @@
         <v>97</v>
       </c>
       <c r="L78" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M78" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N78" s="22" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O78" s="23" t="s">
         <v>25</v>
@@ -5150,25 +5150,25 @@
         <v>78</v>
       </c>
       <c r="B79" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="C79" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D79" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E79" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F79" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G79" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H79" s="19" t="s">
         <v>248</v>
-      </c>
-      <c r="C79" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D79" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E79" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F79" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G79" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H79" s="19" t="s">
-        <v>249</v>
       </c>
       <c r="I79" s="20" t="s">
         <v>54</v>
@@ -5185,7 +5185,7 @@
       </c>
       <c r="M79" s="22"/>
       <c r="N79" s="22" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="O79" s="23" t="s">
         <v>25</v>
@@ -5199,25 +5199,25 @@
         <v>79</v>
       </c>
       <c r="B80" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="C80" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D80" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E80" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F80" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G80" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H80" s="19" t="s">
         <v>251</v>
-      </c>
-      <c r="C80" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D80" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E80" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F80" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G80" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H80" s="19" t="s">
-        <v>252</v>
       </c>
       <c r="I80" s="20" t="s">
         <v>96</v>
@@ -5230,13 +5230,13 @@
         <v>97</v>
       </c>
       <c r="L80" s="22" t="s">
-        <v>98</v>
+        <v>55</v>
       </c>
       <c r="M80" s="22" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="N80" s="22" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="O80" s="23" t="s">
         <v>25</v>
@@ -5250,25 +5250,25 @@
         <v>80</v>
       </c>
       <c r="B81" s="17" t="s">
+        <v>253</v>
+      </c>
+      <c r="C81" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D81" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E81" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F81" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G81" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H81" s="19" t="s">
         <v>254</v>
-      </c>
-      <c r="C81" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D81" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E81" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F81" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G81" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H81" s="19" t="s">
-        <v>255</v>
       </c>
       <c r="I81" s="20" t="s">
         <v>22</v>
@@ -5285,7 +5285,7 @@
       </c>
       <c r="M81" s="22"/>
       <c r="N81" s="22" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="O81" s="23" t="s">
         <v>25</v>
@@ -5299,25 +5299,25 @@
         <v>81</v>
       </c>
       <c r="B82" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="C82" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D82" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E82" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F82" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G82" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H82" s="19" t="s">
         <v>256</v>
-      </c>
-      <c r="C82" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D82" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E82" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F82" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G82" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H82" s="19" t="s">
-        <v>257</v>
       </c>
       <c r="I82" s="20" t="s">
         <v>22</v>
@@ -5334,7 +5334,7 @@
       </c>
       <c r="M82" s="22"/>
       <c r="N82" s="22" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="O82" s="23" t="s">
         <v>25</v>
@@ -5348,25 +5348,25 @@
         <v>82</v>
       </c>
       <c r="B83" s="17" t="s">
+        <v>257</v>
+      </c>
+      <c r="C83" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D83" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E83" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F83" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G83" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H83" s="19" t="s">
         <v>258</v>
-      </c>
-      <c r="C83" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D83" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E83" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F83" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G83" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H83" s="19" t="s">
-        <v>259</v>
       </c>
       <c r="I83" s="20" t="s">
         <v>22</v>
@@ -5383,7 +5383,7 @@
       </c>
       <c r="M83" s="22"/>
       <c r="N83" s="22" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="O83" s="23" t="s">
         <v>25</v>
@@ -5397,25 +5397,25 @@
         <v>83</v>
       </c>
       <c r="B84" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="C84" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D84" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E84" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="F84" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G84" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="H84" s="19" t="s">
         <v>261</v>
-      </c>
-      <c r="C84" s="18" t="s">
-        <v>17</v>
-      </c>
-      <c r="D84" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="E84" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="F84" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="G84" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H84" s="19" t="s">
-        <v>262</v>
       </c>
       <c r="I84" s="20" t="s">
         <v>22</v>
@@ -5432,7 +5432,7 @@
       </c>
       <c r="M84" s="22"/>
       <c r="N84" s="22" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="O84" s="23" t="s">
         <v>25</v>

</xml_diff>